<commit_message>
Correction of metadata errors
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/2017 Projektek/iotables/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\2017 Projektek\iotables\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="587" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{A7678307-2E79-4A02-A7FF-F508EC91DD07}"/>
+  <xr:revisionPtr revIDLastSave="593" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{2446E729-E4F1-4DC1-835A-83F7645CCDF6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{2909AB96-77CF-4A03-A17F-F023092B1853}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6757" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6757" uniqueCount="737">
   <si>
     <t>A</t>
   </si>
@@ -2237,6 +2237,9 @@
   </si>
   <si>
     <t>inventory_valuable_change</t>
+  </si>
+  <si>
+    <t>wholesale_trade_group</t>
   </si>
 </sst>
 </file>
@@ -16164,7 +16167,7 @@
         <v>2</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66:H97" si="2">VALUE(_xlfn.CONCAT(D66,E66,F66,G66))</f>
+        <f t="shared" ref="H66:H87" si="2">VALUE(_xlfn.CONCAT(D66,E66,F66,G66))</f>
         <v>10092</v>
       </c>
       <c r="I66" t="s">
@@ -18897,7 +18900,7 @@
         <v>0</v>
       </c>
       <c r="H157">
-        <f t="shared" ref="H157:H188" si="5">VALUE(_xlfn.CONCAT(D157,E157,F157,G157))</f>
+        <f t="shared" ref="H157:H186" si="5">VALUE(_xlfn.CONCAT(D157,E157,F157,G157))</f>
         <v>20510</v>
       </c>
       <c r="I157" t="s">
@@ -19756,8 +19759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2028A59-D190-4BE7-BF93-1C1CA36FC2A3}">
   <dimension ref="A1:I187"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I187" sqref="A2:I187"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21235,7 +21238,7 @@
         <v>10090</v>
       </c>
       <c r="I50" t="s">
-        <v>590</v>
+        <v>736</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -21265,7 +21268,7 @@
         <v>10091</v>
       </c>
       <c r="I51" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -21295,7 +21298,7 @@
         <v>10092</v>
       </c>
       <c r="I52" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -21325,7 +21328,7 @@
         <v>10093</v>
       </c>
       <c r="I53" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -21355,7 +21358,7 @@
         <v>10101</v>
       </c>
       <c r="I54" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -21385,7 +21388,7 @@
         <v>10102</v>
       </c>
       <c r="I55" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -21415,7 +21418,7 @@
         <v>10103</v>
       </c>
       <c r="I56" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -21445,7 +21448,7 @@
         <v>10104</v>
       </c>
       <c r="I57" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -21475,7 +21478,7 @@
         <v>10105</v>
       </c>
       <c r="I58" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -23619,7 +23622,7 @@
         <v>1</v>
       </c>
       <c r="H130">
-        <f t="shared" ref="H130:H161" si="4">VALUE(_xlfn.CONCAT(D130,E130,F130,G130))</f>
+        <f t="shared" ref="H130:H154" si="4">VALUE(_xlfn.CONCAT(D130,E130,F130,G130))</f>
         <v>10051</v>
       </c>
       <c r="I130" t="s">
@@ -25322,8 +25325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66AA4A9-AB24-42FC-B620-3CE38CD4AD9A}">
   <dimension ref="A1:J758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="L156" sqref="L156:L158"/>
+    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
+      <selection activeCell="C623" sqref="C623"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29073,7 +29076,7 @@
         <v>10105</v>
       </c>
       <c r="J117" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
@@ -31342,7 +31345,7 @@
         <v>0</v>
       </c>
       <c r="I188">
-        <f>VALUE(_xlfn.CONCAT(E188,F188,G188,H188))</f>
+        <f t="shared" ref="I188:I219" si="0">VALUE(_xlfn.CONCAT(E188,F188,G188,H188))</f>
         <v>10010</v>
       </c>
       <c r="J188" t="s">
@@ -31375,7 +31378,7 @@
         <v>1</v>
       </c>
       <c r="I189">
-        <f>VALUE(_xlfn.CONCAT(E189,F189,G189,H189))</f>
+        <f t="shared" si="0"/>
         <v>10011</v>
       </c>
       <c r="J189" t="s">
@@ -31408,7 +31411,7 @@
         <v>2</v>
       </c>
       <c r="I190">
-        <f>VALUE(_xlfn.CONCAT(E190,F190,G190,H190))</f>
+        <f t="shared" si="0"/>
         <v>10012</v>
       </c>
       <c r="J190" t="s">
@@ -31441,7 +31444,7 @@
         <v>3</v>
       </c>
       <c r="I191">
-        <f>VALUE(_xlfn.CONCAT(E191,F191,G191,H191))</f>
+        <f t="shared" si="0"/>
         <v>10013</v>
       </c>
       <c r="J191" t="s">
@@ -31474,7 +31477,7 @@
         <v>3</v>
       </c>
       <c r="I192">
-        <f>VALUE(_xlfn.CONCAT(E192,F192,G192,H192))</f>
+        <f t="shared" si="0"/>
         <v>20003</v>
       </c>
       <c r="J192" t="s">
@@ -31507,7 +31510,7 @@
         <v>1</v>
       </c>
       <c r="I193">
-        <f>VALUE(_xlfn.CONCAT(E193,F193,G193,H193))</f>
+        <f t="shared" si="0"/>
         <v>20001</v>
       </c>
       <c r="J193" t="s">
@@ -31540,7 +31543,7 @@
         <v>1</v>
       </c>
       <c r="I194">
-        <f>VALUE(_xlfn.CONCAT(E194,F194,G194,H194))</f>
+        <f t="shared" si="0"/>
         <v>10021</v>
       </c>
       <c r="J194" t="s">
@@ -31573,7 +31576,7 @@
         <v>0</v>
       </c>
       <c r="I195">
-        <f>VALUE(_xlfn.CONCAT(E195,F195,G195,H195))</f>
+        <f t="shared" si="0"/>
         <v>20590</v>
       </c>
       <c r="J195" t="s">
@@ -31606,7 +31609,7 @@
         <v>1</v>
       </c>
       <c r="I196">
-        <f>VALUE(_xlfn.CONCAT(E196,F196,G196,H196))</f>
+        <f t="shared" si="0"/>
         <v>20411</v>
       </c>
       <c r="J196" t="s">
@@ -31639,7 +31642,7 @@
         <v>1</v>
       </c>
       <c r="I197">
-        <f>VALUE(_xlfn.CONCAT(E197,F197,G197,H197))</f>
+        <f t="shared" si="0"/>
         <v>20421</v>
       </c>
       <c r="J197" t="s">
@@ -31672,7 +31675,7 @@
         <v>0</v>
       </c>
       <c r="I198">
-        <f>VALUE(_xlfn.CONCAT(E198,F198,G198,H198))</f>
+        <f t="shared" si="0"/>
         <v>20510</v>
       </c>
       <c r="J198" t="s">
@@ -31705,7 +31708,7 @@
         <v>0</v>
       </c>
       <c r="I199">
-        <f>VALUE(_xlfn.CONCAT(E199,F199,G199,H199))</f>
+        <f t="shared" si="0"/>
         <v>10020</v>
       </c>
       <c r="J199" t="s">
@@ -31738,7 +31741,7 @@
         <v>1</v>
       </c>
       <c r="I200">
-        <f>VALUE(_xlfn.CONCAT(E200,F200,G200,H200))</f>
+        <f t="shared" si="0"/>
         <v>10031</v>
       </c>
       <c r="J200" t="s">
@@ -31771,7 +31774,7 @@
         <v>2</v>
       </c>
       <c r="I201">
-        <f>VALUE(_xlfn.CONCAT(E201,F201,G201,H201))</f>
+        <f t="shared" si="0"/>
         <v>10032</v>
       </c>
       <c r="J201" t="s">
@@ -31804,7 +31807,7 @@
         <v>3</v>
       </c>
       <c r="I202">
-        <f>VALUE(_xlfn.CONCAT(E202,F202,G202,H202))</f>
+        <f t="shared" si="0"/>
         <v>10033</v>
       </c>
       <c r="J202" t="s">
@@ -31837,7 +31840,7 @@
         <v>4</v>
       </c>
       <c r="I203">
-        <f>VALUE(_xlfn.CONCAT(E203,F203,G203,H203))</f>
+        <f t="shared" si="0"/>
         <v>10034</v>
       </c>
       <c r="J203" t="s">
@@ -31870,7 +31873,7 @@
         <v>5</v>
       </c>
       <c r="I204">
-        <f>VALUE(_xlfn.CONCAT(E204,F204,G204,H204))</f>
+        <f t="shared" si="0"/>
         <v>10035</v>
       </c>
       <c r="J204" t="s">
@@ -31903,7 +31906,7 @@
         <v>6</v>
       </c>
       <c r="I205">
-        <f>VALUE(_xlfn.CONCAT(E205,F205,G205,H205))</f>
+        <f t="shared" si="0"/>
         <v>10036</v>
       </c>
       <c r="J205" t="s">
@@ -31936,7 +31939,7 @@
         <v>7</v>
       </c>
       <c r="I206">
-        <f>VALUE(_xlfn.CONCAT(E206,F206,G206,H206))</f>
+        <f t="shared" si="0"/>
         <v>10037</v>
       </c>
       <c r="J206" t="s">
@@ -31969,7 +31972,7 @@
         <v>8</v>
       </c>
       <c r="I207">
-        <f>VALUE(_xlfn.CONCAT(E207,F207,G207,H207))</f>
+        <f t="shared" si="0"/>
         <v>10038</v>
       </c>
       <c r="J207" t="s">
@@ -32002,7 +32005,7 @@
         <v>9</v>
       </c>
       <c r="I208">
-        <f>VALUE(_xlfn.CONCAT(E208,F208,G208,H208))</f>
+        <f t="shared" si="0"/>
         <v>10039</v>
       </c>
       <c r="J208" t="s">
@@ -32035,7 +32038,7 @@
         <v>1</v>
       </c>
       <c r="I209">
-        <f>VALUE(_xlfn.CONCAT(E209,F209,G209,H209))</f>
+        <f t="shared" si="0"/>
         <v>10041</v>
       </c>
       <c r="J209" t="s">
@@ -32068,7 +32071,7 @@
         <v>2</v>
       </c>
       <c r="I210">
-        <f>VALUE(_xlfn.CONCAT(E210,F210,G210,H210))</f>
+        <f t="shared" si="0"/>
         <v>10042</v>
       </c>
       <c r="J210" t="s">
@@ -32101,7 +32104,7 @@
         <v>3</v>
       </c>
       <c r="I211">
-        <f>VALUE(_xlfn.CONCAT(E211,F211,G211,H211))</f>
+        <f t="shared" si="0"/>
         <v>10043</v>
       </c>
       <c r="J211" t="s">
@@ -32134,7 +32137,7 @@
         <v>4</v>
       </c>
       <c r="I212">
-        <f>VALUE(_xlfn.CONCAT(E212,F212,G212,H212))</f>
+        <f t="shared" si="0"/>
         <v>10044</v>
       </c>
       <c r="J212" t="s">
@@ -32167,7 +32170,7 @@
         <v>5</v>
       </c>
       <c r="I213">
-        <f>VALUE(_xlfn.CONCAT(E213,F213,G213,H213))</f>
+        <f t="shared" si="0"/>
         <v>10045</v>
       </c>
       <c r="J213" t="s">
@@ -32200,7 +32203,7 @@
         <v>6</v>
       </c>
       <c r="I214">
-        <f>VALUE(_xlfn.CONCAT(E214,F214,G214,H214))</f>
+        <f t="shared" si="0"/>
         <v>10046</v>
       </c>
       <c r="J214" t="s">
@@ -32233,7 +32236,7 @@
         <v>7</v>
       </c>
       <c r="I215">
-        <f>VALUE(_xlfn.CONCAT(E215,F215,G215,H215))</f>
+        <f t="shared" si="0"/>
         <v>10047</v>
       </c>
       <c r="J215" t="s">
@@ -32266,7 +32269,7 @@
         <v>8</v>
       </c>
       <c r="I216">
-        <f>VALUE(_xlfn.CONCAT(E216,F216,G216,H216))</f>
+        <f t="shared" si="0"/>
         <v>10048</v>
       </c>
       <c r="J216" t="s">
@@ -32299,7 +32302,7 @@
         <v>9</v>
       </c>
       <c r="I217">
-        <f>VALUE(_xlfn.CONCAT(E217,F217,G217,H217))</f>
+        <f t="shared" si="0"/>
         <v>10049</v>
       </c>
       <c r="J217" t="s">
@@ -32332,7 +32335,7 @@
         <v>1</v>
       </c>
       <c r="I218">
-        <f>VALUE(_xlfn.CONCAT(E218,F218,G218,H218))</f>
+        <f t="shared" si="0"/>
         <v>10051</v>
       </c>
       <c r="J218" t="s">
@@ -32365,7 +32368,7 @@
         <v>0</v>
       </c>
       <c r="I219">
-        <f>VALUE(_xlfn.CONCAT(E219,F219,G219,H219))</f>
+        <f t="shared" si="0"/>
         <v>10010</v>
       </c>
       <c r="J219" t="s">
@@ -32398,7 +32401,7 @@
         <v>1</v>
       </c>
       <c r="I220">
-        <f>VALUE(_xlfn.CONCAT(E220,F220,G220,H220))</f>
+        <f t="shared" ref="I220:I251" si="1">VALUE(_xlfn.CONCAT(E220,F220,G220,H220))</f>
         <v>10011</v>
       </c>
       <c r="J220" t="s">
@@ -32431,7 +32434,7 @@
         <v>2</v>
       </c>
       <c r="I221">
-        <f>VALUE(_xlfn.CONCAT(E221,F221,G221,H221))</f>
+        <f t="shared" si="1"/>
         <v>10012</v>
       </c>
       <c r="J221" t="s">
@@ -32464,7 +32467,7 @@
         <v>3</v>
       </c>
       <c r="I222">
-        <f>VALUE(_xlfn.CONCAT(E222,F222,G222,H222))</f>
+        <f t="shared" si="1"/>
         <v>10013</v>
       </c>
       <c r="J222" t="s">
@@ -32497,7 +32500,7 @@
         <v>1</v>
       </c>
       <c r="I223">
-        <f>VALUE(_xlfn.CONCAT(E223,F223,G223,H223))</f>
+        <f t="shared" si="1"/>
         <v>10021</v>
       </c>
       <c r="J223" t="s">
@@ -32530,7 +32533,7 @@
         <v>0</v>
       </c>
       <c r="I224">
-        <f>VALUE(_xlfn.CONCAT(E224,F224,G224,H224))</f>
+        <f t="shared" si="1"/>
         <v>10020</v>
       </c>
       <c r="J224" t="s">
@@ -32563,7 +32566,7 @@
         <v>1</v>
       </c>
       <c r="I225">
-        <f>VALUE(_xlfn.CONCAT(E225,F225,G225,H225))</f>
+        <f t="shared" si="1"/>
         <v>10031</v>
       </c>
       <c r="J225" t="s">
@@ -32596,7 +32599,7 @@
         <v>2</v>
       </c>
       <c r="I226">
-        <f>VALUE(_xlfn.CONCAT(E226,F226,G226,H226))</f>
+        <f t="shared" si="1"/>
         <v>10032</v>
       </c>
       <c r="J226" t="s">
@@ -32629,7 +32632,7 @@
         <v>3</v>
       </c>
       <c r="I227">
-        <f>VALUE(_xlfn.CONCAT(E227,F227,G227,H227))</f>
+        <f t="shared" si="1"/>
         <v>10033</v>
       </c>
       <c r="J227" t="s">
@@ -32662,7 +32665,7 @@
         <v>4</v>
       </c>
       <c r="I228">
-        <f>VALUE(_xlfn.CONCAT(E228,F228,G228,H228))</f>
+        <f t="shared" si="1"/>
         <v>10034</v>
       </c>
       <c r="J228" t="s">
@@ -32695,7 +32698,7 @@
         <v>5</v>
       </c>
       <c r="I229">
-        <f>VALUE(_xlfn.CONCAT(E229,F229,G229,H229))</f>
+        <f t="shared" si="1"/>
         <v>10035</v>
       </c>
       <c r="J229" t="s">
@@ -32728,7 +32731,7 @@
         <v>6</v>
       </c>
       <c r="I230">
-        <f>VALUE(_xlfn.CONCAT(E230,F230,G230,H230))</f>
+        <f t="shared" si="1"/>
         <v>10036</v>
       </c>
       <c r="J230" t="s">
@@ -32761,7 +32764,7 @@
         <v>7</v>
       </c>
       <c r="I231">
-        <f>VALUE(_xlfn.CONCAT(E231,F231,G231,H231))</f>
+        <f t="shared" si="1"/>
         <v>10037</v>
       </c>
       <c r="J231" t="s">
@@ -32794,7 +32797,7 @@
         <v>8</v>
       </c>
       <c r="I232">
-        <f>VALUE(_xlfn.CONCAT(E232,F232,G232,H232))</f>
+        <f t="shared" si="1"/>
         <v>10038</v>
       </c>
       <c r="J232" t="s">
@@ -32827,7 +32830,7 @@
         <v>9</v>
       </c>
       <c r="I233">
-        <f>VALUE(_xlfn.CONCAT(E233,F233,G233,H233))</f>
+        <f t="shared" si="1"/>
         <v>10039</v>
       </c>
       <c r="J233" t="s">
@@ -32860,7 +32863,7 @@
         <v>1</v>
       </c>
       <c r="I234">
-        <f>VALUE(_xlfn.CONCAT(E234,F234,G234,H234))</f>
+        <f t="shared" si="1"/>
         <v>10041</v>
       </c>
       <c r="J234" t="s">
@@ -32893,7 +32896,7 @@
         <v>2</v>
       </c>
       <c r="I235">
-        <f>VALUE(_xlfn.CONCAT(E235,F235,G235,H235))</f>
+        <f t="shared" si="1"/>
         <v>10042</v>
       </c>
       <c r="J235" t="s">
@@ -32926,7 +32929,7 @@
         <v>3</v>
       </c>
       <c r="I236">
-        <f>VALUE(_xlfn.CONCAT(E236,F236,G236,H236))</f>
+        <f t="shared" si="1"/>
         <v>10043</v>
       </c>
       <c r="J236" t="s">
@@ -32959,7 +32962,7 @@
         <v>4</v>
       </c>
       <c r="I237">
-        <f>VALUE(_xlfn.CONCAT(E237,F237,G237,H237))</f>
+        <f t="shared" si="1"/>
         <v>10044</v>
       </c>
       <c r="J237" t="s">
@@ -32992,7 +32995,7 @@
         <v>5</v>
       </c>
       <c r="I238">
-        <f>VALUE(_xlfn.CONCAT(E238,F238,G238,H238))</f>
+        <f t="shared" si="1"/>
         <v>10045</v>
       </c>
       <c r="J238" t="s">
@@ -33025,7 +33028,7 @@
         <v>6</v>
       </c>
       <c r="I239">
-        <f>VALUE(_xlfn.CONCAT(E239,F239,G239,H239))</f>
+        <f t="shared" si="1"/>
         <v>10046</v>
       </c>
       <c r="J239" t="s">
@@ -33058,7 +33061,7 @@
         <v>7</v>
       </c>
       <c r="I240">
-        <f>VALUE(_xlfn.CONCAT(E240,F240,G240,H240))</f>
+        <f t="shared" si="1"/>
         <v>10047</v>
       </c>
       <c r="J240" t="s">
@@ -33091,7 +33094,7 @@
         <v>8</v>
       </c>
       <c r="I241">
-        <f>VALUE(_xlfn.CONCAT(E241,F241,G241,H241))</f>
+        <f t="shared" si="1"/>
         <v>10048</v>
       </c>
       <c r="J241" t="s">
@@ -33124,7 +33127,7 @@
         <v>9</v>
       </c>
       <c r="I242">
-        <f>VALUE(_xlfn.CONCAT(E242,F242,G242,H242))</f>
+        <f t="shared" si="1"/>
         <v>10049</v>
       </c>
       <c r="J242" t="s">
@@ -33157,7 +33160,7 @@
         <v>1</v>
       </c>
       <c r="I243">
-        <f>VALUE(_xlfn.CONCAT(E243,F243,G243,H243))</f>
+        <f t="shared" si="1"/>
         <v>10051</v>
       </c>
       <c r="J243" t="s">
@@ -33190,7 +33193,7 @@
         <v>0</v>
       </c>
       <c r="I244">
-        <f>VALUE(_xlfn.CONCAT(E244,F244,G244,H244))</f>
+        <f t="shared" si="1"/>
         <v>10060</v>
       </c>
       <c r="J244" t="s">
@@ -33223,7 +33226,7 @@
         <v>1</v>
       </c>
       <c r="I245">
-        <f>VALUE(_xlfn.CONCAT(E245,F245,G245,H245))</f>
+        <f t="shared" si="1"/>
         <v>10071</v>
       </c>
       <c r="J245" t="s">
@@ -33256,7 +33259,7 @@
         <v>2</v>
       </c>
       <c r="I246">
-        <f>VALUE(_xlfn.CONCAT(E246,F246,G246,H246))</f>
+        <f t="shared" si="1"/>
         <v>10072</v>
       </c>
       <c r="J246" t="s">
@@ -33289,7 +33292,7 @@
         <v>0</v>
       </c>
       <c r="I247">
-        <f>VALUE(_xlfn.CONCAT(E247,F247,G247,H247))</f>
+        <f t="shared" si="1"/>
         <v>10080</v>
       </c>
       <c r="J247" t="s">
@@ -33322,7 +33325,7 @@
         <v>1</v>
       </c>
       <c r="I248">
-        <f>VALUE(_xlfn.CONCAT(E248,F248,G248,H248))</f>
+        <f t="shared" si="1"/>
         <v>10091</v>
       </c>
       <c r="J248" t="s">
@@ -33355,7 +33358,7 @@
         <v>2</v>
       </c>
       <c r="I249">
-        <f>VALUE(_xlfn.CONCAT(E249,F249,G249,H249))</f>
+        <f t="shared" si="1"/>
         <v>10092</v>
       </c>
       <c r="J249" t="s">
@@ -33388,7 +33391,7 @@
         <v>3</v>
       </c>
       <c r="I250">
-        <f>VALUE(_xlfn.CONCAT(E250,F250,G250,H250))</f>
+        <f t="shared" si="1"/>
         <v>10093</v>
       </c>
       <c r="J250" t="s">
@@ -33421,7 +33424,7 @@
         <v>0</v>
       </c>
       <c r="I251">
-        <f>VALUE(_xlfn.CONCAT(E251,F251,G251,H251))</f>
+        <f t="shared" si="1"/>
         <v>10090</v>
       </c>
       <c r="J251" t="s">
@@ -33454,7 +33457,7 @@
         <v>1</v>
       </c>
       <c r="I252">
-        <f>VALUE(_xlfn.CONCAT(E252,F252,G252,H252))</f>
+        <f t="shared" ref="I252:I283" si="2">VALUE(_xlfn.CONCAT(E252,F252,G252,H252))</f>
         <v>10101</v>
       </c>
       <c r="J252" t="s">
@@ -33487,7 +33490,7 @@
         <v>2</v>
       </c>
       <c r="I253">
-        <f>VALUE(_xlfn.CONCAT(E253,F253,G253,H253))</f>
+        <f t="shared" si="2"/>
         <v>10102</v>
       </c>
       <c r="J253" t="s">
@@ -33520,7 +33523,7 @@
         <v>3</v>
       </c>
       <c r="I254">
-        <f>VALUE(_xlfn.CONCAT(E254,F254,G254,H254))</f>
+        <f t="shared" si="2"/>
         <v>10103</v>
       </c>
       <c r="J254" t="s">
@@ -33553,7 +33556,7 @@
         <v>4</v>
       </c>
       <c r="I255">
-        <f>VALUE(_xlfn.CONCAT(E255,F255,G255,H255))</f>
+        <f t="shared" si="2"/>
         <v>10104</v>
       </c>
       <c r="J255" t="s">
@@ -33586,7 +33589,7 @@
         <v>5</v>
       </c>
       <c r="I256">
-        <f>VALUE(_xlfn.CONCAT(E256,F256,G256,H256))</f>
+        <f t="shared" si="2"/>
         <v>10105</v>
       </c>
       <c r="J256" t="s">
@@ -33619,7 +33622,7 @@
         <v>0</v>
       </c>
       <c r="I257">
-        <f>VALUE(_xlfn.CONCAT(E257,F257,G257,H257))</f>
+        <f t="shared" si="2"/>
         <v>10110</v>
       </c>
       <c r="J257" t="s">
@@ -33652,7 +33655,7 @@
         <v>0</v>
       </c>
       <c r="I258">
-        <f>VALUE(_xlfn.CONCAT(E258,F258,G258,H258))</f>
+        <f t="shared" si="2"/>
         <v>10120</v>
       </c>
       <c r="J258" t="s">
@@ -33685,7 +33688,7 @@
         <v>1</v>
       </c>
       <c r="I259">
-        <f>VALUE(_xlfn.CONCAT(E259,F259,G259,H259))</f>
+        <f t="shared" si="2"/>
         <v>10121</v>
       </c>
       <c r="J259" t="s">
@@ -33718,7 +33721,7 @@
         <v>2</v>
       </c>
       <c r="I260">
-        <f>VALUE(_xlfn.CONCAT(E260,F260,G260,H260))</f>
+        <f t="shared" si="2"/>
         <v>10122</v>
       </c>
       <c r="J260" t="s">
@@ -33751,7 +33754,7 @@
         <v>3</v>
       </c>
       <c r="I261">
-        <f>VALUE(_xlfn.CONCAT(E261,F261,G261,H261))</f>
+        <f t="shared" si="2"/>
         <v>10123</v>
       </c>
       <c r="J261" t="s">
@@ -33784,7 +33787,7 @@
         <v>4</v>
       </c>
       <c r="I262">
-        <f>VALUE(_xlfn.CONCAT(E262,F262,G262,H262))</f>
+        <f t="shared" si="2"/>
         <v>10124</v>
       </c>
       <c r="J262" t="s">
@@ -33817,7 +33820,7 @@
         <v>0</v>
       </c>
       <c r="I263">
-        <f>VALUE(_xlfn.CONCAT(E263,F263,G263,H263))</f>
+        <f t="shared" si="2"/>
         <v>10130</v>
       </c>
       <c r="J263" t="s">
@@ -33850,7 +33853,7 @@
         <v>1</v>
       </c>
       <c r="I264">
-        <f>VALUE(_xlfn.CONCAT(E264,F264,G264,H264))</f>
+        <f t="shared" si="2"/>
         <v>10131</v>
       </c>
       <c r="J264" t="s">
@@ -33883,7 +33886,7 @@
         <v>2</v>
       </c>
       <c r="I265">
-        <f>VALUE(_xlfn.CONCAT(E265,F265,G265,H265))</f>
+        <f t="shared" si="2"/>
         <v>10132</v>
       </c>
       <c r="J265" t="s">
@@ -33916,7 +33919,7 @@
         <v>3</v>
       </c>
       <c r="I266">
-        <f>VALUE(_xlfn.CONCAT(E266,F266,G266,H266))</f>
+        <f t="shared" si="2"/>
         <v>10133</v>
       </c>
       <c r="J266" t="s">
@@ -33949,7 +33952,7 @@
         <v>0</v>
       </c>
       <c r="I267">
-        <f>VALUE(_xlfn.CONCAT(E267,F267,G267,H267))</f>
+        <f t="shared" si="2"/>
         <v>10140</v>
       </c>
       <c r="J267" t="s">
@@ -34046,7 +34049,7 @@
         <v>0</v>
       </c>
       <c r="I270">
-        <f>VALUE(_xlfn.CONCAT(E270,F270,G270,H270))</f>
+        <f t="shared" ref="I270:I294" si="3">VALUE(_xlfn.CONCAT(E270,F270,G270,H270))</f>
         <v>10150</v>
       </c>
       <c r="J270" t="s">
@@ -34079,7 +34082,7 @@
         <v>1</v>
       </c>
       <c r="I271">
-        <f>VALUE(_xlfn.CONCAT(E271,F271,G271,H271))</f>
+        <f t="shared" si="3"/>
         <v>10151</v>
       </c>
       <c r="J271" t="s">
@@ -34112,7 +34115,7 @@
         <v>2</v>
       </c>
       <c r="I272">
-        <f>VALUE(_xlfn.CONCAT(E272,F272,G272,H272))</f>
+        <f t="shared" si="3"/>
         <v>10152</v>
       </c>
       <c r="J272" t="s">
@@ -34145,7 +34148,7 @@
         <v>3</v>
       </c>
       <c r="I273">
-        <f>VALUE(_xlfn.CONCAT(E273,F273,G273,H273))</f>
+        <f t="shared" si="3"/>
         <v>10153</v>
       </c>
       <c r="J273" t="s">
@@ -34178,7 +34181,7 @@
         <v>4</v>
       </c>
       <c r="I274">
-        <f>VALUE(_xlfn.CONCAT(E274,F274,G274,H274))</f>
+        <f t="shared" si="3"/>
         <v>10154</v>
       </c>
       <c r="J274" t="s">
@@ -34211,7 +34214,7 @@
         <v>5</v>
       </c>
       <c r="I275">
-        <f>VALUE(_xlfn.CONCAT(E275,F275,G275,H275))</f>
+        <f t="shared" si="3"/>
         <v>10155</v>
       </c>
       <c r="J275" t="s">
@@ -34244,7 +34247,7 @@
         <v>1</v>
       </c>
       <c r="I276">
-        <f>VALUE(_xlfn.CONCAT(E276,F276,G276,H276))</f>
+        <f t="shared" si="3"/>
         <v>10161</v>
       </c>
       <c r="J276" t="s">
@@ -34277,7 +34280,7 @@
         <v>2</v>
       </c>
       <c r="I277">
-        <f>VALUE(_xlfn.CONCAT(E277,F277,G277,H277))</f>
+        <f t="shared" si="3"/>
         <v>10162</v>
       </c>
       <c r="J277" t="s">
@@ -34310,7 +34313,7 @@
         <v>3</v>
       </c>
       <c r="I278">
-        <f>VALUE(_xlfn.CONCAT(E278,F278,G278,H278))</f>
+        <f t="shared" si="3"/>
         <v>10163</v>
       </c>
       <c r="J278" t="s">
@@ -34343,7 +34346,7 @@
         <v>4</v>
       </c>
       <c r="I279">
-        <f>VALUE(_xlfn.CONCAT(E279,F279,G279,H279))</f>
+        <f t="shared" si="3"/>
         <v>10164</v>
       </c>
       <c r="J279" t="s">
@@ -34376,7 +34379,7 @@
         <v>1</v>
       </c>
       <c r="I280">
-        <f>VALUE(_xlfn.CONCAT(E280,F280,G280,H280))</f>
+        <f t="shared" si="3"/>
         <v>10171</v>
       </c>
       <c r="J280" t="s">
@@ -34409,7 +34412,7 @@
         <v>0</v>
       </c>
       <c r="I281">
-        <f>VALUE(_xlfn.CONCAT(E281,F281,G281,H281))</f>
+        <f t="shared" si="3"/>
         <v>10170</v>
       </c>
       <c r="J281" t="s">
@@ -34442,7 +34445,7 @@
         <v>0</v>
       </c>
       <c r="I282">
-        <f>VALUE(_xlfn.CONCAT(E282,F282,G282,H282))</f>
+        <f t="shared" si="3"/>
         <v>10180</v>
       </c>
       <c r="J282" t="s">
@@ -34475,7 +34478,7 @@
         <v>0</v>
       </c>
       <c r="I283">
-        <f>VALUE(_xlfn.CONCAT(E283,F283,G283,H283))</f>
+        <f t="shared" si="3"/>
         <v>10190</v>
       </c>
       <c r="J283" t="s">
@@ -34508,7 +34511,7 @@
         <v>0</v>
       </c>
       <c r="I284">
-        <f>VALUE(_xlfn.CONCAT(E284,F284,G284,H284))</f>
+        <f t="shared" si="3"/>
         <v>10190</v>
       </c>
       <c r="J284" t="s">
@@ -34541,7 +34544,7 @@
         <v>1</v>
       </c>
       <c r="I285">
-        <f>VALUE(_xlfn.CONCAT(E285,F285,G285,H285))</f>
+        <f t="shared" si="3"/>
         <v>10191</v>
       </c>
       <c r="J285" t="s">
@@ -34574,7 +34577,7 @@
         <v>1</v>
       </c>
       <c r="I286">
-        <f>VALUE(_xlfn.CONCAT(E286,F286,G286,H286))</f>
+        <f t="shared" si="3"/>
         <v>10201</v>
       </c>
       <c r="J286" t="s">
@@ -34607,7 +34610,7 @@
         <v>2</v>
       </c>
       <c r="I287">
-        <f>VALUE(_xlfn.CONCAT(E287,F287,G287,H287))</f>
+        <f t="shared" si="3"/>
         <v>10202</v>
       </c>
       <c r="J287" t="s">
@@ -34640,7 +34643,7 @@
         <v>0</v>
       </c>
       <c r="I288">
-        <f>VALUE(_xlfn.CONCAT(E288,F288,G288,H288))</f>
+        <f t="shared" si="3"/>
         <v>10200</v>
       </c>
       <c r="J288" t="s">
@@ -34673,7 +34676,7 @@
         <v>2</v>
       </c>
       <c r="I289">
-        <f>VALUE(_xlfn.CONCAT(E289,F289,G289,H289))</f>
+        <f t="shared" si="3"/>
         <v>10212</v>
       </c>
       <c r="J289" t="s">
@@ -34706,7 +34709,7 @@
         <v>3</v>
       </c>
       <c r="I290">
-        <f>VALUE(_xlfn.CONCAT(E290,F290,G290,H290))</f>
+        <f t="shared" si="3"/>
         <v>10213</v>
       </c>
       <c r="J290" t="s">
@@ -34739,7 +34742,7 @@
         <v>0</v>
       </c>
       <c r="I291">
-        <f>VALUE(_xlfn.CONCAT(E291,F291,G291,H291))</f>
+        <f t="shared" si="3"/>
         <v>10220</v>
       </c>
       <c r="J291" t="s">
@@ -34772,7 +34775,7 @@
         <v>0</v>
       </c>
       <c r="I292">
-        <f>VALUE(_xlfn.CONCAT(E292,F292,G292,H292))</f>
+        <f t="shared" si="3"/>
         <v>10230</v>
       </c>
       <c r="J292" t="s">
@@ -34805,7 +34808,7 @@
         <v>0</v>
       </c>
       <c r="I293">
-        <f>VALUE(_xlfn.CONCAT(E293,F293,G293,H293))</f>
+        <f t="shared" si="3"/>
         <v>10240</v>
       </c>
       <c r="J293" t="s">
@@ -34838,7 +34841,7 @@
         <v>0</v>
       </c>
       <c r="I294">
-        <f>VALUE(_xlfn.CONCAT(E294,F294,G294,H294))</f>
+        <f t="shared" si="3"/>
         <v>10060</v>
       </c>
       <c r="J294" t="s">
@@ -34903,7 +34906,7 @@
         <v>2</v>
       </c>
       <c r="I296">
-        <f>VALUE(_xlfn.CONCAT(E296,F296,G296,H296))</f>
+        <f t="shared" ref="I296:I323" si="4">VALUE(_xlfn.CONCAT(E296,F296,G296,H296))</f>
         <v>20112</v>
       </c>
       <c r="J296" t="s">
@@ -34936,7 +34939,7 @@
         <v>0</v>
       </c>
       <c r="I297">
-        <f>VALUE(_xlfn.CONCAT(E297,F297,G297,H297))</f>
+        <f t="shared" si="4"/>
         <v>30830</v>
       </c>
       <c r="J297" t="s">
@@ -34969,7 +34972,7 @@
         <v>0</v>
       </c>
       <c r="I298">
-        <f>VALUE(_xlfn.CONCAT(E298,F298,G298,H298))</f>
+        <f t="shared" si="4"/>
         <v>20220</v>
       </c>
       <c r="J298" t="s">
@@ -35002,7 +35005,7 @@
         <v>1</v>
       </c>
       <c r="I299">
-        <f>VALUE(_xlfn.CONCAT(E299,F299,G299,H299))</f>
+        <f t="shared" si="4"/>
         <v>10071</v>
       </c>
       <c r="J299" t="s">
@@ -35035,7 +35038,7 @@
         <v>2</v>
       </c>
       <c r="I300">
-        <f>VALUE(_xlfn.CONCAT(E300,F300,G300,H300))</f>
+        <f t="shared" si="4"/>
         <v>10072</v>
       </c>
       <c r="J300" t="s">
@@ -35068,7 +35071,7 @@
         <v>1</v>
       </c>
       <c r="I301">
-        <f>VALUE(_xlfn.CONCAT(E301,F301,G301,H301))</f>
+        <f t="shared" si="4"/>
         <v>50101</v>
       </c>
       <c r="J301" t="s">
@@ -35101,7 +35104,7 @@
         <v>0</v>
       </c>
       <c r="I302">
-        <f>VALUE(_xlfn.CONCAT(E302,F302,G302,H302))</f>
+        <f t="shared" si="4"/>
         <v>10080</v>
       </c>
       <c r="J302" t="s">
@@ -35134,7 +35137,7 @@
         <v>1</v>
       </c>
       <c r="I303">
-        <f>VALUE(_xlfn.CONCAT(E303,F303,G303,H303))</f>
+        <f t="shared" si="4"/>
         <v>10091</v>
       </c>
       <c r="J303" t="s">
@@ -35167,7 +35170,7 @@
         <v>2</v>
       </c>
       <c r="I304">
-        <f>VALUE(_xlfn.CONCAT(E304,F304,G304,H304))</f>
+        <f t="shared" si="4"/>
         <v>10092</v>
       </c>
       <c r="J304" t="s">
@@ -35200,7 +35203,7 @@
         <v>3</v>
       </c>
       <c r="I305">
-        <f>VALUE(_xlfn.CONCAT(E305,F305,G305,H305))</f>
+        <f t="shared" si="4"/>
         <v>10093</v>
       </c>
       <c r="J305" t="s">
@@ -35233,7 +35236,7 @@
         <v>0</v>
       </c>
       <c r="I306">
-        <f>VALUE(_xlfn.CONCAT(E306,F306,G306,H306))</f>
+        <f t="shared" si="4"/>
         <v>10090</v>
       </c>
       <c r="J306" t="s">
@@ -35266,7 +35269,7 @@
         <v>1</v>
       </c>
       <c r="I307">
-        <f>VALUE(_xlfn.CONCAT(E307,F307,G307,H307))</f>
+        <f t="shared" si="4"/>
         <v>10101</v>
       </c>
       <c r="J307" t="s">
@@ -35299,7 +35302,7 @@
         <v>2</v>
       </c>
       <c r="I308">
-        <f>VALUE(_xlfn.CONCAT(E308,F308,G308,H308))</f>
+        <f t="shared" si="4"/>
         <v>10102</v>
       </c>
       <c r="J308" t="s">
@@ -35332,7 +35335,7 @@
         <v>3</v>
       </c>
       <c r="I309">
-        <f>VALUE(_xlfn.CONCAT(E309,F309,G309,H309))</f>
+        <f t="shared" si="4"/>
         <v>10103</v>
       </c>
       <c r="J309" t="s">
@@ -35365,7 +35368,7 @@
         <v>4</v>
       </c>
       <c r="I310">
-        <f>VALUE(_xlfn.CONCAT(E310,F310,G310,H310))</f>
+        <f t="shared" si="4"/>
         <v>10104</v>
       </c>
       <c r="J310" t="s">
@@ -35398,7 +35401,7 @@
         <v>5</v>
       </c>
       <c r="I311">
-        <f>VALUE(_xlfn.CONCAT(E311,F311,G311,H311))</f>
+        <f t="shared" si="4"/>
         <v>10105</v>
       </c>
       <c r="J311" t="s">
@@ -35431,7 +35434,7 @@
         <v>0</v>
       </c>
       <c r="I312">
-        <f>VALUE(_xlfn.CONCAT(E312,F312,G312,H312))</f>
+        <f t="shared" si="4"/>
         <v>10110</v>
       </c>
       <c r="J312" t="s">
@@ -35464,7 +35467,7 @@
         <v>0</v>
       </c>
       <c r="I313">
-        <f>VALUE(_xlfn.CONCAT(E313,F313,G313,H313))</f>
+        <f t="shared" si="4"/>
         <v>20750</v>
       </c>
       <c r="J313" t="s">
@@ -35497,7 +35500,7 @@
         <v>0</v>
       </c>
       <c r="I314">
-        <f>VALUE(_xlfn.CONCAT(E314,F314,G314,H314))</f>
+        <f t="shared" si="4"/>
         <v>10120</v>
       </c>
       <c r="J314" t="s">
@@ -35530,7 +35533,7 @@
         <v>1</v>
       </c>
       <c r="I315">
-        <f>VALUE(_xlfn.CONCAT(E315,F315,G315,H315))</f>
+        <f t="shared" si="4"/>
         <v>10121</v>
       </c>
       <c r="J315" t="s">
@@ -35563,7 +35566,7 @@
         <v>2</v>
       </c>
       <c r="I316">
-        <f>VALUE(_xlfn.CONCAT(E316,F316,G316,H316))</f>
+        <f t="shared" si="4"/>
         <v>10122</v>
       </c>
       <c r="J316" t="s">
@@ -35596,7 +35599,7 @@
         <v>3</v>
       </c>
       <c r="I317">
-        <f>VALUE(_xlfn.CONCAT(E317,F317,G317,H317))</f>
+        <f t="shared" si="4"/>
         <v>10123</v>
       </c>
       <c r="J317" t="s">
@@ -35629,7 +35632,7 @@
         <v>4</v>
       </c>
       <c r="I318">
-        <f>VALUE(_xlfn.CONCAT(E318,F318,G318,H318))</f>
+        <f t="shared" si="4"/>
         <v>10124</v>
       </c>
       <c r="J318" t="s">
@@ -35662,7 +35665,7 @@
         <v>0</v>
       </c>
       <c r="I319">
-        <f>VALUE(_xlfn.CONCAT(E319,F319,G319,H319))</f>
+        <f t="shared" si="4"/>
         <v>10130</v>
       </c>
       <c r="J319" t="s">
@@ -35695,7 +35698,7 @@
         <v>1</v>
       </c>
       <c r="I320">
-        <f>VALUE(_xlfn.CONCAT(E320,F320,G320,H320))</f>
+        <f t="shared" si="4"/>
         <v>10131</v>
       </c>
       <c r="J320" t="s">
@@ -35728,7 +35731,7 @@
         <v>2</v>
       </c>
       <c r="I321">
-        <f>VALUE(_xlfn.CONCAT(E321,F321,G321,H321))</f>
+        <f t="shared" si="4"/>
         <v>10132</v>
       </c>
       <c r="J321" t="s">
@@ -35761,7 +35764,7 @@
         <v>3</v>
       </c>
       <c r="I322">
-        <f>VALUE(_xlfn.CONCAT(E322,F322,G322,H322))</f>
+        <f t="shared" si="4"/>
         <v>10133</v>
       </c>
       <c r="J322" t="s">
@@ -35794,7 +35797,7 @@
         <v>0</v>
       </c>
       <c r="I323">
-        <f>VALUE(_xlfn.CONCAT(E323,F323,G323,H323))</f>
+        <f t="shared" si="4"/>
         <v>10140</v>
       </c>
       <c r="J323" t="s">
@@ -35891,7 +35894,7 @@
         <v>0</v>
       </c>
       <c r="I326">
-        <f>VALUE(_xlfn.CONCAT(E326,F326,G326,H326))</f>
+        <f t="shared" ref="I326:I343" si="5">VALUE(_xlfn.CONCAT(E326,F326,G326,H326))</f>
         <v>50900</v>
       </c>
       <c r="J326" t="s">
@@ -35924,7 +35927,7 @@
         <v>0</v>
       </c>
       <c r="I327">
-        <f>VALUE(_xlfn.CONCAT(E327,F327,G327,H327))</f>
+        <f t="shared" si="5"/>
         <v>10150</v>
       </c>
       <c r="J327" t="s">
@@ -35957,7 +35960,7 @@
         <v>1</v>
       </c>
       <c r="I328">
-        <f>VALUE(_xlfn.CONCAT(E328,F328,G328,H328))</f>
+        <f t="shared" si="5"/>
         <v>10151</v>
       </c>
       <c r="J328" t="s">
@@ -35990,7 +35993,7 @@
         <v>2</v>
       </c>
       <c r="I329">
-        <f>VALUE(_xlfn.CONCAT(E329,F329,G329,H329))</f>
+        <f t="shared" si="5"/>
         <v>10152</v>
       </c>
       <c r="J329" t="s">
@@ -36023,7 +36026,7 @@
         <v>3</v>
       </c>
       <c r="I330">
-        <f>VALUE(_xlfn.CONCAT(E330,F330,G330,H330))</f>
+        <f t="shared" si="5"/>
         <v>10153</v>
       </c>
       <c r="J330" t="s">
@@ -36056,7 +36059,7 @@
         <v>4</v>
       </c>
       <c r="I331">
-        <f>VALUE(_xlfn.CONCAT(E331,F331,G331,H331))</f>
+        <f t="shared" si="5"/>
         <v>10154</v>
       </c>
       <c r="J331" t="s">
@@ -36089,7 +36092,7 @@
         <v>5</v>
       </c>
       <c r="I332">
-        <f>VALUE(_xlfn.CONCAT(E332,F332,G332,H332))</f>
+        <f t="shared" si="5"/>
         <v>10155</v>
       </c>
       <c r="J332" t="s">
@@ -36122,7 +36125,7 @@
         <v>1</v>
       </c>
       <c r="I333">
-        <f>VALUE(_xlfn.CONCAT(E333,F333,G333,H333))</f>
+        <f t="shared" si="5"/>
         <v>10161</v>
       </c>
       <c r="J333" t="s">
@@ -36155,7 +36158,7 @@
         <v>2</v>
       </c>
       <c r="I334">
-        <f>VALUE(_xlfn.CONCAT(E334,F334,G334,H334))</f>
+        <f t="shared" si="5"/>
         <v>10162</v>
       </c>
       <c r="J334" t="s">
@@ -36188,7 +36191,7 @@
         <v>3</v>
       </c>
       <c r="I335">
-        <f>VALUE(_xlfn.CONCAT(E335,F335,G335,H335))</f>
+        <f t="shared" si="5"/>
         <v>10163</v>
       </c>
       <c r="J335" t="s">
@@ -36221,7 +36224,7 @@
         <v>4</v>
       </c>
       <c r="I336">
-        <f>VALUE(_xlfn.CONCAT(E336,F336,G336,H336))</f>
+        <f t="shared" si="5"/>
         <v>10164</v>
       </c>
       <c r="J336" t="s">
@@ -36254,7 +36257,7 @@
         <v>9</v>
       </c>
       <c r="I337">
-        <f>VALUE(_xlfn.CONCAT(E337,F337,G337,H337))</f>
+        <f t="shared" si="5"/>
         <v>99999</v>
       </c>
       <c r="J337" t="s">
@@ -36287,7 +36290,7 @@
         <v>1</v>
       </c>
       <c r="I338">
-        <f>VALUE(_xlfn.CONCAT(E338,F338,G338,H338))</f>
+        <f t="shared" si="5"/>
         <v>10171</v>
       </c>
       <c r="J338" t="s">
@@ -36320,7 +36323,7 @@
         <v>4</v>
       </c>
       <c r="I339">
-        <f>VALUE(_xlfn.CONCAT(E339,F339,G339,H339))</f>
+        <f t="shared" si="5"/>
         <v>20004</v>
       </c>
       <c r="J339" t="s">
@@ -36353,7 +36356,7 @@
         <v>2</v>
       </c>
       <c r="I340">
-        <f>VALUE(_xlfn.CONCAT(E340,F340,G340,H340))</f>
+        <f t="shared" si="5"/>
         <v>20002</v>
       </c>
       <c r="J340" t="s">
@@ -36386,7 +36389,7 @@
         <v>0</v>
       </c>
       <c r="I341">
-        <f>VALUE(_xlfn.CONCAT(E341,F341,G341,H341))</f>
+        <f t="shared" si="5"/>
         <v>10170</v>
       </c>
       <c r="J341" t="s">
@@ -36419,7 +36422,7 @@
         <v>0</v>
       </c>
       <c r="I342">
-        <f>VALUE(_xlfn.CONCAT(E342,F342,G342,H342))</f>
+        <f t="shared" si="5"/>
         <v>10180</v>
       </c>
       <c r="J342" t="s">
@@ -36452,7 +36455,7 @@
         <v>0</v>
       </c>
       <c r="I343">
-        <f>VALUE(_xlfn.CONCAT(E343,F343,G343,H343))</f>
+        <f t="shared" si="5"/>
         <v>20690</v>
       </c>
       <c r="J343" t="s">
@@ -36581,7 +36584,7 @@
         <v>0</v>
       </c>
       <c r="I347">
-        <f>VALUE(_xlfn.CONCAT(E347,F347,G347,H347))</f>
+        <f t="shared" ref="I347:I367" si="6">VALUE(_xlfn.CONCAT(E347,F347,G347,H347))</f>
         <v>20090</v>
       </c>
       <c r="J347" t="s">
@@ -36614,7 +36617,7 @@
         <v>1</v>
       </c>
       <c r="I348">
-        <f>VALUE(_xlfn.CONCAT(E348,F348,G348,H348))</f>
+        <f t="shared" si="6"/>
         <v>30091</v>
       </c>
       <c r="J348" t="s">
@@ -36647,7 +36650,7 @@
         <v>0</v>
       </c>
       <c r="I349">
-        <f>VALUE(_xlfn.CONCAT(E349,F349,G349,H349))</f>
+        <f t="shared" si="6"/>
         <v>20310</v>
       </c>
       <c r="J349" t="s">
@@ -36680,7 +36683,7 @@
         <v>0</v>
       </c>
       <c r="I350">
-        <f>VALUE(_xlfn.CONCAT(E350,F350,G350,H350))</f>
+        <f t="shared" si="6"/>
         <v>30590</v>
       </c>
       <c r="J350" t="s">
@@ -36713,7 +36716,7 @@
         <v>9</v>
       </c>
       <c r="I351">
-        <f>VALUE(_xlfn.CONCAT(E351,F351,G351,H351))</f>
+        <f t="shared" si="6"/>
         <v>20079</v>
       </c>
       <c r="J351" t="s">
@@ -36746,7 +36749,7 @@
         <v>4</v>
       </c>
       <c r="I352">
-        <f>VALUE(_xlfn.CONCAT(E352,F352,G352,H352))</f>
+        <f t="shared" si="6"/>
         <v>20074</v>
       </c>
       <c r="J352" t="s">
@@ -36779,7 +36782,7 @@
         <v>7</v>
       </c>
       <c r="I353">
-        <f>VALUE(_xlfn.CONCAT(E353,F353,G353,H353))</f>
+        <f t="shared" si="6"/>
         <v>20077</v>
       </c>
       <c r="J353" t="s">
@@ -36812,7 +36815,7 @@
         <v>5</v>
       </c>
       <c r="I354">
-        <f>VALUE(_xlfn.CONCAT(E354,F354,G354,H354))</f>
+        <f t="shared" si="6"/>
         <v>20075</v>
       </c>
       <c r="J354" t="s">
@@ -36845,7 +36848,7 @@
         <v>6</v>
       </c>
       <c r="I355">
-        <f>VALUE(_xlfn.CONCAT(E355,F355,G355,H355))</f>
+        <f t="shared" si="6"/>
         <v>20076</v>
       </c>
       <c r="J355" t="s">
@@ -36878,7 +36881,7 @@
         <v>0</v>
       </c>
       <c r="I356">
-        <f>VALUE(_xlfn.CONCAT(E356,F356,G356,H356))</f>
+        <f t="shared" si="6"/>
         <v>10190</v>
       </c>
       <c r="J356" t="s">
@@ -36911,7 +36914,7 @@
         <v>1</v>
       </c>
       <c r="I357">
-        <f>VALUE(_xlfn.CONCAT(E357,F357,G357,H357))</f>
+        <f t="shared" si="6"/>
         <v>10191</v>
       </c>
       <c r="J357" t="s">
@@ -36944,7 +36947,7 @@
         <v>1</v>
       </c>
       <c r="I358">
-        <f>VALUE(_xlfn.CONCAT(E358,F358,G358,H358))</f>
+        <f t="shared" si="6"/>
         <v>10201</v>
       </c>
       <c r="J358" t="s">
@@ -36977,7 +36980,7 @@
         <v>2</v>
       </c>
       <c r="I359">
-        <f>VALUE(_xlfn.CONCAT(E359,F359,G359,H359))</f>
+        <f t="shared" si="6"/>
         <v>10202</v>
       </c>
       <c r="J359" t="s">
@@ -37010,7 +37013,7 @@
         <v>0</v>
       </c>
       <c r="I360">
-        <f>VALUE(_xlfn.CONCAT(E360,F360,G360,H360))</f>
+        <f t="shared" si="6"/>
         <v>10200</v>
       </c>
       <c r="J360" t="s">
@@ -37043,7 +37046,7 @@
         <v>1</v>
       </c>
       <c r="I361">
-        <f>VALUE(_xlfn.CONCAT(E361,F361,G361,H361))</f>
+        <f t="shared" si="6"/>
         <v>10211</v>
       </c>
       <c r="J361" t="s">
@@ -37076,7 +37079,7 @@
         <v>2</v>
       </c>
       <c r="I362">
-        <f>VALUE(_xlfn.CONCAT(E362,F362,G362,H362))</f>
+        <f t="shared" si="6"/>
         <v>10212</v>
       </c>
       <c r="J362" t="s">
@@ -37109,7 +37112,7 @@
         <v>3</v>
       </c>
       <c r="I363">
-        <f>VALUE(_xlfn.CONCAT(E363,F363,G363,H363))</f>
+        <f t="shared" si="6"/>
         <v>10213</v>
       </c>
       <c r="J363" t="s">
@@ -37142,7 +37145,7 @@
         <v>0</v>
       </c>
       <c r="I364">
-        <f>VALUE(_xlfn.CONCAT(E364,F364,G364,H364))</f>
+        <f t="shared" si="6"/>
         <v>10230</v>
       </c>
       <c r="J364" t="s">
@@ -37175,7 +37178,7 @@
         <v>0</v>
       </c>
       <c r="I365">
-        <f>VALUE(_xlfn.CONCAT(E365,F365,G365,H365))</f>
+        <f t="shared" si="6"/>
         <v>20010</v>
       </c>
       <c r="J365" t="s">
@@ -37208,7 +37211,7 @@
         <v>0</v>
       </c>
       <c r="I366">
-        <f>VALUE(_xlfn.CONCAT(E366,F366,G366,H366))</f>
+        <f t="shared" si="6"/>
         <v>10300</v>
       </c>
       <c r="J366" t="s">
@@ -37241,7 +37244,7 @@
         <v>1</v>
       </c>
       <c r="I367">
-        <f>VALUE(_xlfn.CONCAT(E367,F367,G367,H367))</f>
+        <f t="shared" si="6"/>
         <v>30891</v>
       </c>
       <c r="J367" t="s">

</xml_diff>

<commit_message>
chasing typo in real_estate_services_b
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\2017 Projektek\iotables\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\_package\iotables\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="593" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{2446E729-E4F1-4DC1-835A-83F7645CCDF6}"/>
+  <xr:revisionPtr revIDLastSave="595" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{6AB0DEC3-0365-479E-A66E-1F25F73E6A0D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{2909AB96-77CF-4A03-A17F-F023092B1853}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="induse" sheetId="3" r:id="rId4"/>
     <sheet name="all" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6757" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6757" uniqueCount="739">
   <si>
     <t>A</t>
   </si>
@@ -2240,6 +2240,12 @@
   </si>
   <si>
     <t>wholesale_trade_group</t>
+  </si>
+  <si>
+    <t>real_estate_services</t>
+  </si>
+  <si>
+    <t>real_estate_services_b</t>
   </si>
 </sst>
 </file>
@@ -25325,8 +25331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66AA4A9-AB24-42FC-B620-3CE38CD4AD9A}">
   <dimension ref="A1:J758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="C623" sqref="C623"/>
+    <sheetView tabSelected="1" topLeftCell="A626" workbookViewId="0">
+      <selection activeCell="J637" sqref="J637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27860,7 +27866,7 @@
         <v>10142</v>
       </c>
       <c r="J79" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -29492,7 +29498,7 @@
         <v>10142</v>
       </c>
       <c r="J130" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -33457,7 +33463,7 @@
         <v>1</v>
       </c>
       <c r="I252">
-        <f t="shared" ref="I252:I283" si="2">VALUE(_xlfn.CONCAT(E252,F252,G252,H252))</f>
+        <f t="shared" ref="I252:I267" si="2">VALUE(_xlfn.CONCAT(E252,F252,G252,H252))</f>
         <v>10101</v>
       </c>
       <c r="J252" t="s">
@@ -34020,7 +34026,7 @@
         <v>10142</v>
       </c>
       <c r="J269" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
@@ -35865,7 +35871,7 @@
         <v>10142</v>
       </c>
       <c r="J325" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.25">
@@ -39809,7 +39815,7 @@
         <v>10142</v>
       </c>
       <c r="J447" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.25">
@@ -41537,7 +41543,7 @@
         <v>10142</v>
       </c>
       <c r="J501" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="502" spans="1:10" x14ac:dyDescent="0.25">
@@ -45793,7 +45799,7 @@
         <v>10140</v>
       </c>
       <c r="J634" t="s">
-        <v>652</v>
+        <v>737</v>
       </c>
     </row>
     <row r="635" spans="1:10" x14ac:dyDescent="0.25">
@@ -45889,7 +45895,7 @@
         <v>10142</v>
       </c>
       <c r="J637" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.25">
@@ -47841,7 +47847,7 @@
         <v>10142</v>
       </c>
       <c r="J698" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="699" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correcting a vocubulary error
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://visegradinvestments-my.sharepoint.com/personal/antaldaniel_visegradinvestments_onmicrosoft_com/Documents/_package/iotables/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Antal\OneDrive - Visegrad Investments\_package\iotables\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{BEBBC1ED-6F14-4CAB-868A-5958479E2D37}"/>
+  <xr:revisionPtr revIDLastSave="636" documentId="BBCC240E134AA52ED9EF656885D7EABF48622902" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{C8CD28D1-8E0A-4B8B-B288-5F175C503F09}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4" xr2:uid="{2909AB96-77CF-4A03-A17F-F023092B1853}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">t_cols!$A$1:$I$186</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6780" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6780" uniqueCount="741">
   <si>
     <t>A</t>
   </si>
@@ -2257,6 +2258,9 @@
   </si>
   <si>
     <t>Computer programming, consultancy and related services;Information services</t>
+  </si>
+  <si>
+    <t>intermediate_consumption_total</t>
   </si>
 </sst>
 </file>
@@ -8715,7 +8719,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H205">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H205">
     <sortCondition ref="D2:D205"/>
     <sortCondition ref="E2:E205"/>
   </sortState>
@@ -14224,7 +14228,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I184">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I184">
     <sortCondition ref="H2:H184"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19797,7 +19801,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I186">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I186">
     <sortCondition ref="H2:H186"/>
     <sortCondition ref="E2:E186"/>
   </sortState>
@@ -25393,7 +25397,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H188">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H188">
     <sortCondition ref="A2:A188"/>
     <sortCondition ref="H2:H188"/>
   </sortState>
@@ -25405,8 +25409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66AA4A9-AB24-42FC-B620-3CE38CD4AD9A}">
   <dimension ref="A1:J761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="D263" sqref="D263"/>
+    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="J349" sqref="J349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36701,7 +36705,7 @@
         <v>20090</v>
       </c>
       <c r="J348" t="s">
-        <v>604</v>
+        <v>658</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
@@ -36734,7 +36738,7 @@
         <v>30091</v>
       </c>
       <c r="J349" t="s">
-        <v>658</v>
+        <v>740</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.25">
@@ -49942,7 +49946,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J761">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J761">
     <sortCondition ref="A2:A761"/>
     <sortCondition ref="C2:C761"/>
   </sortState>

</xml_diff>